<commit_message>
sincronizado todo desde otra carpeta local, con base en GH del 22/08. Se incorpora 03-procesamiento_fuentesAngela con flextable acordadas con Martin
</commit_message>
<xml_diff>
--- a/data/tablas03.xlsx
+++ b/data/tablas03.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://msair-my.sharepoint.com/personal/arojas_air_org/Documents/Documents/testsidil/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arojas\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="418" documentId="8_{9BF37307-FEEC-4BA2-897C-EAB5562178B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50A69DD6-4867-494E-9715-7A54AC0AC57B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D2BD6C-343F-4E82-8944-F98255D0A2A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="10" xr2:uid="{DBF64252-CF13-48F0-ABAE-2D362372F5FC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="12" xr2:uid="{DBF64252-CF13-48F0-ABAE-2D362372F5FC}"/>
   </bookViews>
   <sheets>
     <sheet name="tabla1" sheetId="12" r:id="rId1"/>
@@ -24,6 +24,8 @@
     <sheet name="tabla9" sheetId="20" r:id="rId9"/>
     <sheet name="tabla10" sheetId="10" r:id="rId10"/>
     <sheet name="tabla11" sheetId="21" r:id="rId11"/>
+    <sheet name="tabla12" sheetId="22" r:id="rId12"/>
+    <sheet name="tabla13" sheetId="23" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="308">
   <si>
     <t>Fuente</t>
   </si>
@@ -916,6 +918,60 @@
   </si>
   <si>
     <t>Script de configuración inicial:  0_config_inicial</t>
+  </si>
+  <si>
+    <t>inspeccion</t>
+  </si>
+  <si>
+    <t>submateria_id</t>
+  </si>
+  <si>
+    <t>d_viol_procede</t>
+  </si>
+  <si>
+    <t>in_anio</t>
+  </si>
+  <si>
+    <t>contrato_escrito</t>
+  </si>
+  <si>
+    <t>brecha_imss</t>
+  </si>
+  <si>
+    <t>otros indicadores….</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>CENTRO_trabajo_:id</t>
+  </si>
+  <si>
+    <t>inspeccion_id</t>
+  </si>
+  <si>
+    <t>d_vio_procede3</t>
+  </si>
+  <si>
+    <t>d_vio_procede4</t>
+  </si>
+  <si>
+    <t>d_vio_procede5</t>
+  </si>
+  <si>
+    <t>d_vio_procede7</t>
+  </si>
+  <si>
+    <t>d_vio_procede8</t>
+  </si>
+  <si>
+    <t>d_viopocede100154</t>
+  </si>
+  <si>
+    <t>NaN</t>
+  </si>
+  <si>
+    <t>d_vio_procede912</t>
   </si>
 </sst>
 </file>
@@ -986,7 +1042,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1004,6 +1060,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2221,7 +2281,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BFF4A2D-03C2-4699-995B-C479F1BE0198}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
@@ -2325,6 +2385,944 @@
       <c r="D6" t="s">
         <v>252</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38437E6F-1194-4BB4-9533-DB462EADA4F0}">
+  <dimension ref="A1:M11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.5546875" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="B1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="F1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G1" t="s">
+        <v>207</v>
+      </c>
+      <c r="H1" t="s">
+        <v>201</v>
+      </c>
+      <c r="I1" t="s">
+        <v>203</v>
+      </c>
+      <c r="J1" t="s">
+        <v>198</v>
+      </c>
+      <c r="K1" t="s">
+        <v>294</v>
+      </c>
+      <c r="L1" t="s">
+        <v>295</v>
+      </c>
+      <c r="M1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>5450</v>
+      </c>
+      <c r="B2">
+        <v>10001</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2017</v>
+      </c>
+      <c r="F2">
+        <v>11</v>
+      </c>
+      <c r="G2">
+        <v>113</v>
+      </c>
+      <c r="H2">
+        <v>23</v>
+      </c>
+      <c r="I2">
+        <v>23001</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>0.45</v>
+      </c>
+      <c r="L2">
+        <v>0.54</v>
+      </c>
+      <c r="M2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>5450</v>
+      </c>
+      <c r="B3">
+        <v>10001</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>2017</v>
+      </c>
+      <c r="F3">
+        <v>11</v>
+      </c>
+      <c r="G3">
+        <v>113</v>
+      </c>
+      <c r="H3">
+        <v>23</v>
+      </c>
+      <c r="I3">
+        <v>23001</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>0.45</v>
+      </c>
+      <c r="L3">
+        <v>0.54</v>
+      </c>
+      <c r="M3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>5450</v>
+      </c>
+      <c r="B4">
+        <v>10001</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>2017</v>
+      </c>
+      <c r="F4">
+        <v>11</v>
+      </c>
+      <c r="G4">
+        <v>113</v>
+      </c>
+      <c r="H4">
+        <v>23</v>
+      </c>
+      <c r="I4">
+        <v>23001</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>0.45</v>
+      </c>
+      <c r="L4">
+        <v>0.54</v>
+      </c>
+      <c r="M4" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>5450</v>
+      </c>
+      <c r="B5">
+        <v>1231154</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>2021</v>
+      </c>
+      <c r="F5">
+        <v>11</v>
+      </c>
+      <c r="G5">
+        <v>113</v>
+      </c>
+      <c r="H5">
+        <v>23</v>
+      </c>
+      <c r="I5">
+        <v>23001</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <v>0.64</v>
+      </c>
+      <c r="L5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="M5" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5450</v>
+      </c>
+      <c r="B6">
+        <v>1231154</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>2021</v>
+      </c>
+      <c r="F6">
+        <v>11</v>
+      </c>
+      <c r="G6">
+        <v>113</v>
+      </c>
+      <c r="H6">
+        <v>23</v>
+      </c>
+      <c r="I6">
+        <v>23001</v>
+      </c>
+      <c r="J6">
+        <v>2</v>
+      </c>
+      <c r="K6">
+        <v>0.64</v>
+      </c>
+      <c r="L6">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="M6" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5450</v>
+      </c>
+      <c r="B7">
+        <v>1231154</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>2021</v>
+      </c>
+      <c r="F7">
+        <v>11</v>
+      </c>
+      <c r="G7">
+        <v>113</v>
+      </c>
+      <c r="H7">
+        <v>23</v>
+      </c>
+      <c r="I7">
+        <v>23001</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>0.64</v>
+      </c>
+      <c r="L7">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="M7" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>8888</v>
+      </c>
+      <c r="B8">
+        <v>54564</v>
+      </c>
+      <c r="C8">
+        <v>25</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>2012</v>
+      </c>
+      <c r="F8">
+        <v>35</v>
+      </c>
+      <c r="G8">
+        <v>356</v>
+      </c>
+      <c r="H8">
+        <v>32</v>
+      </c>
+      <c r="I8">
+        <v>32001</v>
+      </c>
+      <c r="J8">
+        <v>4</v>
+      </c>
+      <c r="K8">
+        <v>0.23</v>
+      </c>
+      <c r="L8">
+        <v>0.2</v>
+      </c>
+      <c r="M8" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>9999</v>
+      </c>
+      <c r="B9">
+        <v>2447</v>
+      </c>
+      <c r="C9">
+        <v>36</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>2019</v>
+      </c>
+      <c r="F9">
+        <v>84</v>
+      </c>
+      <c r="G9">
+        <v>841</v>
+      </c>
+      <c r="H9">
+        <v>10</v>
+      </c>
+      <c r="I9">
+        <v>10015</v>
+      </c>
+      <c r="J9">
+        <v>5</v>
+      </c>
+      <c r="K9">
+        <v>0.05</v>
+      </c>
+      <c r="L9">
+        <v>0.6</v>
+      </c>
+      <c r="M9" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>12154</v>
+      </c>
+      <c r="B10">
+        <v>244</v>
+      </c>
+      <c r="C10">
+        <v>25</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>2022</v>
+      </c>
+      <c r="F10">
+        <v>91</v>
+      </c>
+      <c r="G10">
+        <v>911</v>
+      </c>
+      <c r="H10">
+        <v>11</v>
+      </c>
+      <c r="I10">
+        <v>11121</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>0.99</v>
+      </c>
+      <c r="L10">
+        <v>0.4</v>
+      </c>
+      <c r="M10" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>32134</v>
+      </c>
+      <c r="B11">
+        <v>3277</v>
+      </c>
+      <c r="C11">
+        <v>99</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>2018</v>
+      </c>
+      <c r="F11">
+        <v>21</v>
+      </c>
+      <c r="G11">
+        <v>213</v>
+      </c>
+      <c r="H11">
+        <v>12</v>
+      </c>
+      <c r="I11">
+        <v>12005</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>0.8</v>
+      </c>
+      <c r="L11">
+        <v>0.85</v>
+      </c>
+      <c r="M11" t="s">
+        <v>297</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2469070-095E-4BE2-8A18-4BDD272BB645}">
+  <dimension ref="A1:R11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="K1" t="s">
+        <v>205</v>
+      </c>
+      <c r="L1" t="s">
+        <v>207</v>
+      </c>
+      <c r="M1" t="s">
+        <v>201</v>
+      </c>
+      <c r="N1" t="s">
+        <v>203</v>
+      </c>
+      <c r="O1" t="s">
+        <v>198</v>
+      </c>
+      <c r="P1" t="s">
+        <v>294</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>295</v>
+      </c>
+      <c r="R1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>5450</v>
+      </c>
+      <c r="B2" s="7">
+        <v>10001</v>
+      </c>
+      <c r="C2" s="7">
+        <v>2012</v>
+      </c>
+      <c r="D2" s="7">
+        <v>1</v>
+      </c>
+      <c r="E2" s="7">
+        <v>0</v>
+      </c>
+      <c r="F2" s="7">
+        <v>1</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="K2">
+        <v>11</v>
+      </c>
+      <c r="L2">
+        <v>113</v>
+      </c>
+      <c r="M2">
+        <v>23</v>
+      </c>
+      <c r="N2">
+        <v>23001</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>0.45</v>
+      </c>
+      <c r="Q2">
+        <v>0.23</v>
+      </c>
+      <c r="R2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <v>222</v>
+      </c>
+      <c r="B3" s="7">
+        <v>1231154</v>
+      </c>
+      <c r="C3" s="7">
+        <v>2019</v>
+      </c>
+      <c r="D3" s="7">
+        <v>1</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="F3" s="7">
+        <v>1</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0</v>
+      </c>
+      <c r="H3" s="7">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="K3">
+        <v>33</v>
+      </c>
+      <c r="L3" t="s">
+        <v>306</v>
+      </c>
+      <c r="M3">
+        <v>15</v>
+      </c>
+      <c r="N3">
+        <v>15003</v>
+      </c>
+      <c r="O3">
+        <v>6</v>
+      </c>
+      <c r="P3">
+        <v>0.78</v>
+      </c>
+      <c r="Q3">
+        <v>0.54</v>
+      </c>
+      <c r="R3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>32134</v>
+      </c>
+      <c r="B4" s="7">
+        <v>54564</v>
+      </c>
+      <c r="C4" s="7">
+        <v>2020</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1</v>
+      </c>
+      <c r="F4" s="7">
+        <v>0</v>
+      </c>
+      <c r="G4" s="7">
+        <v>1</v>
+      </c>
+      <c r="H4" s="7">
+        <v>0</v>
+      </c>
+      <c r="I4" s="7">
+        <v>0</v>
+      </c>
+      <c r="J4" s="7">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>43</v>
+      </c>
+      <c r="L4">
+        <v>433</v>
+      </c>
+      <c r="M4">
+        <v>31</v>
+      </c>
+      <c r="N4">
+        <v>31008</v>
+      </c>
+      <c r="O4">
+        <v>3</v>
+      </c>
+      <c r="P4">
+        <v>0.38</v>
+      </c>
+      <c r="Q4">
+        <v>0.46</v>
+      </c>
+      <c r="R4" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>444</v>
+      </c>
+      <c r="B5" s="7">
+        <v>2447</v>
+      </c>
+      <c r="C5" s="7">
+        <v>2015</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0</v>
+      </c>
+      <c r="E5" s="7">
+        <v>1</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="H5" s="7">
+        <v>1</v>
+      </c>
+      <c r="I5" s="7">
+        <v>1</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>48</v>
+      </c>
+      <c r="L5">
+        <v>484</v>
+      </c>
+      <c r="M5">
+        <v>11</v>
+      </c>
+      <c r="N5" t="s">
+        <v>306</v>
+      </c>
+      <c r="O5" t="s">
+        <v>306</v>
+      </c>
+      <c r="P5">
+        <v>0.63</v>
+      </c>
+      <c r="Q5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="R5" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>12154</v>
+      </c>
+      <c r="B6" s="7">
+        <v>244</v>
+      </c>
+      <c r="C6" s="7">
+        <v>2023</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="I6" s="7">
+        <v>0</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="K6">
+        <v>11</v>
+      </c>
+      <c r="L6">
+        <v>112</v>
+      </c>
+      <c r="M6">
+        <v>28</v>
+      </c>
+      <c r="N6">
+        <v>28006</v>
+      </c>
+      <c r="O6">
+        <v>2</v>
+      </c>
+      <c r="P6">
+        <v>0.54</v>
+      </c>
+      <c r="Q6">
+        <v>0.65</v>
+      </c>
+      <c r="R6" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>12154</v>
+      </c>
+      <c r="B7" s="7">
+        <v>3277</v>
+      </c>
+      <c r="C7" s="7">
+        <v>2017</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="7">
+        <v>1</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="J7" s="7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>11</v>
+      </c>
+      <c r="L7">
+        <v>112</v>
+      </c>
+      <c r="M7">
+        <v>28</v>
+      </c>
+      <c r="N7">
+        <v>28006</v>
+      </c>
+      <c r="O7">
+        <v>2</v>
+      </c>
+      <c r="P7">
+        <v>0.65</v>
+      </c>
+      <c r="Q7">
+        <v>0.34</v>
+      </c>
+      <c r="R7" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Incorporo primeros cambios de Martín y equipo DGIET a capítulos 01, 02 y 04, y tablas 03 y 04.
</commit_message>
<xml_diff>
--- a/data/tablas03.xlsx
+++ b/data/tablas03.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://msair-my.sharepoint.com/personal/arojas_air_org/Documents/Documents/testsidil/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arojas\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="418" documentId="8_{9BF37307-FEEC-4BA2-897C-EAB5562178B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50A69DD6-4867-494E-9715-7A54AC0AC57B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D2BD6C-343F-4E82-8944-F98255D0A2A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="10" xr2:uid="{DBF64252-CF13-48F0-ABAE-2D362372F5FC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="12" xr2:uid="{DBF64252-CF13-48F0-ABAE-2D362372F5FC}"/>
   </bookViews>
   <sheets>
     <sheet name="tabla1" sheetId="12" r:id="rId1"/>
@@ -24,6 +24,8 @@
     <sheet name="tabla9" sheetId="20" r:id="rId9"/>
     <sheet name="tabla10" sheetId="10" r:id="rId10"/>
     <sheet name="tabla11" sheetId="21" r:id="rId11"/>
+    <sheet name="tabla12" sheetId="22" r:id="rId12"/>
+    <sheet name="tabla13" sheetId="23" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="308">
   <si>
     <t>Fuente</t>
   </si>
@@ -916,6 +918,60 @@
   </si>
   <si>
     <t>Script de configuración inicial:  0_config_inicial</t>
+  </si>
+  <si>
+    <t>inspeccion</t>
+  </si>
+  <si>
+    <t>submateria_id</t>
+  </si>
+  <si>
+    <t>d_viol_procede</t>
+  </si>
+  <si>
+    <t>in_anio</t>
+  </si>
+  <si>
+    <t>contrato_escrito</t>
+  </si>
+  <si>
+    <t>brecha_imss</t>
+  </si>
+  <si>
+    <t>otros indicadores….</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>CENTRO_trabajo_:id</t>
+  </si>
+  <si>
+    <t>inspeccion_id</t>
+  </si>
+  <si>
+    <t>d_vio_procede3</t>
+  </si>
+  <si>
+    <t>d_vio_procede4</t>
+  </si>
+  <si>
+    <t>d_vio_procede5</t>
+  </si>
+  <si>
+    <t>d_vio_procede7</t>
+  </si>
+  <si>
+    <t>d_vio_procede8</t>
+  </si>
+  <si>
+    <t>d_viopocede100154</t>
+  </si>
+  <si>
+    <t>NaN</t>
+  </si>
+  <si>
+    <t>d_vio_procede912</t>
   </si>
 </sst>
 </file>
@@ -986,7 +1042,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1004,6 +1060,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2221,7 +2281,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BFF4A2D-03C2-4699-995B-C479F1BE0198}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
@@ -2325,6 +2385,944 @@
       <c r="D6" t="s">
         <v>252</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38437E6F-1194-4BB4-9533-DB462EADA4F0}">
+  <dimension ref="A1:M11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.5546875" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="B1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="F1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G1" t="s">
+        <v>207</v>
+      </c>
+      <c r="H1" t="s">
+        <v>201</v>
+      </c>
+      <c r="I1" t="s">
+        <v>203</v>
+      </c>
+      <c r="J1" t="s">
+        <v>198</v>
+      </c>
+      <c r="K1" t="s">
+        <v>294</v>
+      </c>
+      <c r="L1" t="s">
+        <v>295</v>
+      </c>
+      <c r="M1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>5450</v>
+      </c>
+      <c r="B2">
+        <v>10001</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2017</v>
+      </c>
+      <c r="F2">
+        <v>11</v>
+      </c>
+      <c r="G2">
+        <v>113</v>
+      </c>
+      <c r="H2">
+        <v>23</v>
+      </c>
+      <c r="I2">
+        <v>23001</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>0.45</v>
+      </c>
+      <c r="L2">
+        <v>0.54</v>
+      </c>
+      <c r="M2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>5450</v>
+      </c>
+      <c r="B3">
+        <v>10001</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>2017</v>
+      </c>
+      <c r="F3">
+        <v>11</v>
+      </c>
+      <c r="G3">
+        <v>113</v>
+      </c>
+      <c r="H3">
+        <v>23</v>
+      </c>
+      <c r="I3">
+        <v>23001</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>0.45</v>
+      </c>
+      <c r="L3">
+        <v>0.54</v>
+      </c>
+      <c r="M3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>5450</v>
+      </c>
+      <c r="B4">
+        <v>10001</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>2017</v>
+      </c>
+      <c r="F4">
+        <v>11</v>
+      </c>
+      <c r="G4">
+        <v>113</v>
+      </c>
+      <c r="H4">
+        <v>23</v>
+      </c>
+      <c r="I4">
+        <v>23001</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>0.45</v>
+      </c>
+      <c r="L4">
+        <v>0.54</v>
+      </c>
+      <c r="M4" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>5450</v>
+      </c>
+      <c r="B5">
+        <v>1231154</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>2021</v>
+      </c>
+      <c r="F5">
+        <v>11</v>
+      </c>
+      <c r="G5">
+        <v>113</v>
+      </c>
+      <c r="H5">
+        <v>23</v>
+      </c>
+      <c r="I5">
+        <v>23001</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <v>0.64</v>
+      </c>
+      <c r="L5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="M5" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5450</v>
+      </c>
+      <c r="B6">
+        <v>1231154</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>2021</v>
+      </c>
+      <c r="F6">
+        <v>11</v>
+      </c>
+      <c r="G6">
+        <v>113</v>
+      </c>
+      <c r="H6">
+        <v>23</v>
+      </c>
+      <c r="I6">
+        <v>23001</v>
+      </c>
+      <c r="J6">
+        <v>2</v>
+      </c>
+      <c r="K6">
+        <v>0.64</v>
+      </c>
+      <c r="L6">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="M6" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5450</v>
+      </c>
+      <c r="B7">
+        <v>1231154</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>2021</v>
+      </c>
+      <c r="F7">
+        <v>11</v>
+      </c>
+      <c r="G7">
+        <v>113</v>
+      </c>
+      <c r="H7">
+        <v>23</v>
+      </c>
+      <c r="I7">
+        <v>23001</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>0.64</v>
+      </c>
+      <c r="L7">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="M7" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>8888</v>
+      </c>
+      <c r="B8">
+        <v>54564</v>
+      </c>
+      <c r="C8">
+        <v>25</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>2012</v>
+      </c>
+      <c r="F8">
+        <v>35</v>
+      </c>
+      <c r="G8">
+        <v>356</v>
+      </c>
+      <c r="H8">
+        <v>32</v>
+      </c>
+      <c r="I8">
+        <v>32001</v>
+      </c>
+      <c r="J8">
+        <v>4</v>
+      </c>
+      <c r="K8">
+        <v>0.23</v>
+      </c>
+      <c r="L8">
+        <v>0.2</v>
+      </c>
+      <c r="M8" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>9999</v>
+      </c>
+      <c r="B9">
+        <v>2447</v>
+      </c>
+      <c r="C9">
+        <v>36</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>2019</v>
+      </c>
+      <c r="F9">
+        <v>84</v>
+      </c>
+      <c r="G9">
+        <v>841</v>
+      </c>
+      <c r="H9">
+        <v>10</v>
+      </c>
+      <c r="I9">
+        <v>10015</v>
+      </c>
+      <c r="J9">
+        <v>5</v>
+      </c>
+      <c r="K9">
+        <v>0.05</v>
+      </c>
+      <c r="L9">
+        <v>0.6</v>
+      </c>
+      <c r="M9" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>12154</v>
+      </c>
+      <c r="B10">
+        <v>244</v>
+      </c>
+      <c r="C10">
+        <v>25</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>2022</v>
+      </c>
+      <c r="F10">
+        <v>91</v>
+      </c>
+      <c r="G10">
+        <v>911</v>
+      </c>
+      <c r="H10">
+        <v>11</v>
+      </c>
+      <c r="I10">
+        <v>11121</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>0.99</v>
+      </c>
+      <c r="L10">
+        <v>0.4</v>
+      </c>
+      <c r="M10" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>32134</v>
+      </c>
+      <c r="B11">
+        <v>3277</v>
+      </c>
+      <c r="C11">
+        <v>99</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>2018</v>
+      </c>
+      <c r="F11">
+        <v>21</v>
+      </c>
+      <c r="G11">
+        <v>213</v>
+      </c>
+      <c r="H11">
+        <v>12</v>
+      </c>
+      <c r="I11">
+        <v>12005</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>0.8</v>
+      </c>
+      <c r="L11">
+        <v>0.85</v>
+      </c>
+      <c r="M11" t="s">
+        <v>297</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2469070-095E-4BE2-8A18-4BDD272BB645}">
+  <dimension ref="A1:R11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="K1" t="s">
+        <v>205</v>
+      </c>
+      <c r="L1" t="s">
+        <v>207</v>
+      </c>
+      <c r="M1" t="s">
+        <v>201</v>
+      </c>
+      <c r="N1" t="s">
+        <v>203</v>
+      </c>
+      <c r="O1" t="s">
+        <v>198</v>
+      </c>
+      <c r="P1" t="s">
+        <v>294</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>295</v>
+      </c>
+      <c r="R1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>5450</v>
+      </c>
+      <c r="B2" s="7">
+        <v>10001</v>
+      </c>
+      <c r="C2" s="7">
+        <v>2012</v>
+      </c>
+      <c r="D2" s="7">
+        <v>1</v>
+      </c>
+      <c r="E2" s="7">
+        <v>0</v>
+      </c>
+      <c r="F2" s="7">
+        <v>1</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="K2">
+        <v>11</v>
+      </c>
+      <c r="L2">
+        <v>113</v>
+      </c>
+      <c r="M2">
+        <v>23</v>
+      </c>
+      <c r="N2">
+        <v>23001</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>0.45</v>
+      </c>
+      <c r="Q2">
+        <v>0.23</v>
+      </c>
+      <c r="R2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <v>222</v>
+      </c>
+      <c r="B3" s="7">
+        <v>1231154</v>
+      </c>
+      <c r="C3" s="7">
+        <v>2019</v>
+      </c>
+      <c r="D3" s="7">
+        <v>1</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="F3" s="7">
+        <v>1</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0</v>
+      </c>
+      <c r="H3" s="7">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="K3">
+        <v>33</v>
+      </c>
+      <c r="L3" t="s">
+        <v>306</v>
+      </c>
+      <c r="M3">
+        <v>15</v>
+      </c>
+      <c r="N3">
+        <v>15003</v>
+      </c>
+      <c r="O3">
+        <v>6</v>
+      </c>
+      <c r="P3">
+        <v>0.78</v>
+      </c>
+      <c r="Q3">
+        <v>0.54</v>
+      </c>
+      <c r="R3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>32134</v>
+      </c>
+      <c r="B4" s="7">
+        <v>54564</v>
+      </c>
+      <c r="C4" s="7">
+        <v>2020</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1</v>
+      </c>
+      <c r="F4" s="7">
+        <v>0</v>
+      </c>
+      <c r="G4" s="7">
+        <v>1</v>
+      </c>
+      <c r="H4" s="7">
+        <v>0</v>
+      </c>
+      <c r="I4" s="7">
+        <v>0</v>
+      </c>
+      <c r="J4" s="7">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>43</v>
+      </c>
+      <c r="L4">
+        <v>433</v>
+      </c>
+      <c r="M4">
+        <v>31</v>
+      </c>
+      <c r="N4">
+        <v>31008</v>
+      </c>
+      <c r="O4">
+        <v>3</v>
+      </c>
+      <c r="P4">
+        <v>0.38</v>
+      </c>
+      <c r="Q4">
+        <v>0.46</v>
+      </c>
+      <c r="R4" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>444</v>
+      </c>
+      <c r="B5" s="7">
+        <v>2447</v>
+      </c>
+      <c r="C5" s="7">
+        <v>2015</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0</v>
+      </c>
+      <c r="E5" s="7">
+        <v>1</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="H5" s="7">
+        <v>1</v>
+      </c>
+      <c r="I5" s="7">
+        <v>1</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>48</v>
+      </c>
+      <c r="L5">
+        <v>484</v>
+      </c>
+      <c r="M5">
+        <v>11</v>
+      </c>
+      <c r="N5" t="s">
+        <v>306</v>
+      </c>
+      <c r="O5" t="s">
+        <v>306</v>
+      </c>
+      <c r="P5">
+        <v>0.63</v>
+      </c>
+      <c r="Q5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="R5" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>12154</v>
+      </c>
+      <c r="B6" s="7">
+        <v>244</v>
+      </c>
+      <c r="C6" s="7">
+        <v>2023</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="I6" s="7">
+        <v>0</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="K6">
+        <v>11</v>
+      </c>
+      <c r="L6">
+        <v>112</v>
+      </c>
+      <c r="M6">
+        <v>28</v>
+      </c>
+      <c r="N6">
+        <v>28006</v>
+      </c>
+      <c r="O6">
+        <v>2</v>
+      </c>
+      <c r="P6">
+        <v>0.54</v>
+      </c>
+      <c r="Q6">
+        <v>0.65</v>
+      </c>
+      <c r="R6" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>12154</v>
+      </c>
+      <c r="B7" s="7">
+        <v>3277</v>
+      </c>
+      <c r="C7" s="7">
+        <v>2017</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="7">
+        <v>1</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="J7" s="7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>11</v>
+      </c>
+      <c r="L7">
+        <v>112</v>
+      </c>
+      <c r="M7">
+        <v>28</v>
+      </c>
+      <c r="N7">
+        <v>28006</v>
+      </c>
+      <c r="O7">
+        <v>2</v>
+      </c>
+      <c r="P7">
+        <v>0.65</v>
+      </c>
+      <c r="Q7">
+        <v>0.34</v>
+      </c>
+      <c r="R7" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
cambios varios de cara a la version final. Quedan algunos comentarios cancelados de su impresion
</commit_message>
<xml_diff>
--- a/data/tablas03.xlsx
+++ b/data/tablas03.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arojas\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdamerau\Downloads\ManualSIDIL2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D2BD6C-343F-4E82-8944-F98255D0A2A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A4513E-79A6-4F77-8B92-66EEBF9CB365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="12" xr2:uid="{DBF64252-CF13-48F0-ABAE-2D362372F5FC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="2" xr2:uid="{DBF64252-CF13-48F0-ABAE-2D362372F5FC}"/>
   </bookViews>
   <sheets>
     <sheet name="tabla1" sheetId="12" r:id="rId1"/>
@@ -224,9 +224,6 @@
     <t>Posibles mensajes de error o advertencia</t>
   </si>
   <si>
-    <t>Script secuenciador: 1_C_1_S_SE_ENOE</t>
-  </si>
-  <si>
     <t>Declaración de parámetros en la RAM</t>
   </si>
   <si>
@@ -317,9 +314,6 @@
     <t>Principales mensajes confirmatorios esperados[1]</t>
   </si>
   <si>
-    <t>Script secuenciador: 1_secuenciador_IMSS_v.R</t>
-  </si>
-  <si>
     <t>“Hora sistema. INFO: Se ha ejecutado con éxito el script 0_config_inicial.R"</t>
   </si>
   <si>
@@ -539,9 +533,6 @@
     <t>Posibles mensajes de error</t>
   </si>
   <si>
-    <t>Script secuenciador: 1_secuenciador_CENSO2019_v.R</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
@@ -972,6 +963,15 @@
   </si>
   <si>
     <t>d_vio_procede912</t>
+  </si>
+  <si>
+    <t>Script secuenciador: 1_secuenciador_CENSO2019_aaaa_mm_dd.R</t>
+  </si>
+  <si>
+    <t>Script secuenciador: 1_secuenciador_IMSS_aaaa_mm_dd.R</t>
+  </si>
+  <si>
+    <t>Script secuenciador: 1_C_1_S_SE_ENOE_aaaa_mm_dd</t>
   </si>
 </sst>
 </file>
@@ -1384,9 +1384,9 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1403,9 +1403,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -1420,7 +1420,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1454,7 +1454,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1471,7 +1471,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="E8" t="s">
         <v>23</v>
@@ -1535,52 +1535,52 @@
       <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:11" ht="24" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D2" s="3">
         <v>202204</v>
@@ -1592,30 +1592,30 @@
         <v>44.5</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="I2" s="5">
         <v>22</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="K2" s="5">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="24" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D3" s="3">
         <v>202204</v>
@@ -1630,27 +1630,27 @@
         <v>11</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="24" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D4" s="3">
         <v>202204</v>
@@ -1662,30 +1662,30 @@
         <v>57.66</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="K4" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="36" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D5" s="3">
         <v>202204</v>
@@ -1712,15 +1712,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="36" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D6" s="3">
         <v>202204</v>
@@ -1735,27 +1735,27 @@
         <v>11</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="I6" s="5">
         <v>22</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="K6" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="24" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D7" s="3">
         <v>202204</v>
@@ -1773,24 +1773,24 @@
         <v>111</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="24" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D8" s="3">
         <v>202204</v>
@@ -1802,30 +1802,30 @@
         <v>81.78</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="I8" s="5">
         <v>11</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="24" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D9" s="3">
         <v>202204</v>
@@ -1837,10 +1837,10 @@
         <v>84.89</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="I9" s="5">
         <v>31</v>
@@ -1849,18 +1849,18 @@
         <v>31054</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="36" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D10" s="3">
         <v>202204</v>
@@ -1875,27 +1875,27 @@
         <v>43</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="K10" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="36" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D11" s="3">
         <v>202204</v>
@@ -1922,15 +1922,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="36" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D12" s="3">
         <v>202204</v>
@@ -1945,7 +1945,7 @@
         <v>61</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="I12" s="5">
         <v>8</v>
@@ -1957,15 +1957,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="48" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="48" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D13" s="3">
         <v>202204</v>
@@ -1983,27 +1983,27 @@
         <v>613</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="36" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E14" s="2">
         <v>0.71</v>
@@ -2018,27 +2018,27 @@
         <v>313</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="36" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E15" s="2">
         <v>0.56000000000000005</v>
@@ -2047,33 +2047,33 @@
         <v>19.170000000000002</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="I15" s="5">
         <v>25</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="36" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E16" s="2">
         <v>0.18</v>
@@ -2082,10 +2082,10 @@
         <v>71.16</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="I16" s="5">
         <v>24</v>
@@ -2094,21 +2094,21 @@
         <v>24012</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="36" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E17" s="2">
         <v>0.67</v>
@@ -2120,30 +2120,30 @@
         <v>93</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="36" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E18" s="2">
         <v>0.05</v>
@@ -2155,30 +2155,30 @@
         <v>83</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="I18" s="5">
         <v>27</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="K18" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="36" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E19" s="2">
         <v>0.85</v>
@@ -2187,33 +2187,33 @@
         <v>76.45</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="I19" s="5">
         <v>8</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="K19" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="24" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E20" s="2">
         <v>0.44</v>
@@ -2222,33 +2222,33 @@
         <v>31.4</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="I20" s="5">
         <v>1</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="36" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="36" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E21" s="2">
         <v>0.85</v>
@@ -2260,13 +2260,13 @@
         <v>11</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="K21" s="5">
         <v>5</v>
@@ -2285,9 +2285,9 @@
       <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -2298,92 +2298,92 @@
         <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B3" t="s">
+        <v>286</v>
+      </c>
+      <c r="C3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" t="s">
         <v>242</v>
       </c>
-      <c r="B2" t="s">
-        <v>289</v>
-      </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>239</v>
+      </c>
+      <c r="B4" t="s">
         <v>243</v>
       </c>
-      <c r="D2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>242</v>
-      </c>
-      <c r="B3" t="s">
-        <v>289</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>244</v>
       </c>
-      <c r="D3" t="s">
-        <v>90</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D4" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>242</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
         <v>246</v>
       </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B5" t="s">
+        <v>243</v>
+      </c>
+      <c r="C5" t="s">
+        <v>244</v>
+      </c>
+      <c r="D5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>239</v>
+      </c>
+      <c r="B6" t="s">
         <v>247</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C6" t="s">
         <v>248</v>
       </c>
-      <c r="E4" t="s">
+      <c r="D6" t="s">
         <v>249</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>242</v>
-      </c>
-      <c r="B5" t="s">
-        <v>246</v>
-      </c>
-      <c r="C5" t="s">
-        <v>247</v>
-      </c>
-      <c r="D5" t="s">
-        <v>248</v>
-      </c>
-      <c r="E5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>242</v>
-      </c>
-      <c r="B6" t="s">
-        <v>250</v>
-      </c>
-      <c r="C6" t="s">
-        <v>251</v>
-      </c>
-      <c r="D6" t="s">
-        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -2399,60 +2399,60 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.5546875" customWidth="1"/>
-    <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.54296875" customWidth="1"/>
+    <col min="4" max="4" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>290</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1" t="s">
+        <v>200</v>
+      </c>
+      <c r="J1" t="s">
+        <v>195</v>
+      </c>
+      <c r="K1" t="s">
         <v>291</v>
       </c>
-      <c r="D1" t="s">
+      <c r="L1" t="s">
         <v>292</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="M1" t="s">
         <v>293</v>
       </c>
-      <c r="F1" t="s">
-        <v>205</v>
-      </c>
-      <c r="G1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H1" t="s">
-        <v>201</v>
-      </c>
-      <c r="I1" t="s">
-        <v>203</v>
-      </c>
-      <c r="J1" t="s">
-        <v>198</v>
-      </c>
-      <c r="K1" t="s">
-        <v>294</v>
-      </c>
-      <c r="L1" t="s">
-        <v>295</v>
-      </c>
-      <c r="M1" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>5450</v>
       </c>
@@ -2490,10 +2490,10 @@
         <v>0.54</v>
       </c>
       <c r="M2" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>5450</v>
       </c>
@@ -2531,10 +2531,10 @@
         <v>0.54</v>
       </c>
       <c r="M3" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>5450</v>
       </c>
@@ -2572,10 +2572,10 @@
         <v>0.54</v>
       </c>
       <c r="M4" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>5450</v>
       </c>
@@ -2613,10 +2613,10 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="M5" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5450</v>
       </c>
@@ -2654,10 +2654,10 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="M6" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5450</v>
       </c>
@@ -2695,10 +2695,10 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="M7" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>8888</v>
       </c>
@@ -2736,10 +2736,10 @@
         <v>0.2</v>
       </c>
       <c r="M8" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>9999</v>
       </c>
@@ -2777,10 +2777,10 @@
         <v>0.6</v>
       </c>
       <c r="M9" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>12154</v>
       </c>
@@ -2818,10 +2818,10 @@
         <v>0.4</v>
       </c>
       <c r="M10" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>32134</v>
       </c>
@@ -2859,7 +2859,7 @@
         <v>0.85</v>
       </c>
       <c r="M11" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>
@@ -2871,76 +2871,76 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2469070-095E-4BE2-8A18-4BDD272BB645}">
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="G1" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="K1" t="s">
+        <v>202</v>
+      </c>
+      <c r="L1" t="s">
+        <v>204</v>
+      </c>
+      <c r="M1" t="s">
+        <v>198</v>
+      </c>
+      <c r="N1" t="s">
+        <v>200</v>
+      </c>
+      <c r="O1" t="s">
+        <v>195</v>
+      </c>
+      <c r="P1" t="s">
+        <v>291</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>292</v>
+      </c>
+      <c r="R1" t="s">
         <v>293</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>300</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>305</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="K1" t="s">
-        <v>205</v>
-      </c>
-      <c r="L1" t="s">
-        <v>207</v>
-      </c>
-      <c r="M1" t="s">
-        <v>201</v>
-      </c>
-      <c r="N1" t="s">
-        <v>203</v>
-      </c>
-      <c r="O1" t="s">
-        <v>198</v>
-      </c>
-      <c r="P1" t="s">
-        <v>294</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>295</v>
-      </c>
-      <c r="R1" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>5450</v>
       </c>
@@ -2960,16 +2960,16 @@
         <v>1</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="K2">
         <v>11</v>
@@ -2993,10 +2993,10 @@
         <v>0.23</v>
       </c>
       <c r="R2" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="7">
         <v>222</v>
       </c>
@@ -3010,7 +3010,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="F3" s="7">
         <v>1</v>
@@ -3022,16 +3022,16 @@
         <v>0</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="K3">
         <v>33</v>
       </c>
       <c r="L3" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="M3">
         <v>15</v>
@@ -3049,10 +3049,10 @@
         <v>0.54</v>
       </c>
       <c r="R3" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>32134</v>
       </c>
@@ -3063,7 +3063,7 @@
         <v>2020</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="E4" s="7">
         <v>1</v>
@@ -3105,10 +3105,10 @@
         <v>0.46</v>
       </c>
       <c r="R4" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="7">
         <v>444</v>
       </c>
@@ -3125,10 +3125,10 @@
         <v>1</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="H5" s="7">
         <v>1</v>
@@ -3149,10 +3149,10 @@
         <v>11</v>
       </c>
       <c r="N5" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="O5" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="P5">
         <v>0.63</v>
@@ -3161,10 +3161,10 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="R5" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>12154</v>
       </c>
@@ -3175,25 +3175,25 @@
         <v>2023</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="I6" s="7">
         <v>0</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="K6">
         <v>11</v>
@@ -3217,10 +3217,10 @@
         <v>0.65</v>
       </c>
       <c r="R6" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>12154</v>
       </c>
@@ -3243,10 +3243,10 @@
         <v>1</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="J7" s="7">
         <v>1</v>
@@ -3273,10 +3273,10 @@
         <v>0.34</v>
       </c>
       <c r="R7" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -3288,7 +3288,7 @@
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
@@ -3300,7 +3300,7 @@
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -3312,7 +3312,7 @@
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -3337,9 +3337,9 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -3353,7 +3353,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -3361,13 +3361,13 @@
         <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -3375,13 +3375,13 @@
         <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -3395,7 +3395,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -3403,13 +3403,13 @@
         <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -3417,13 +3417,13 @@
         <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -3431,13 +3431,13 @@
         <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -3445,13 +3445,13 @@
         <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -3459,13 +3459,13 @@
         <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -3473,13 +3473,13 @@
         <v>47</v>
       </c>
       <c r="C10" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -3487,13 +3487,13 @@
         <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -3501,7 +3501,7 @@
         <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D12" t="s">
         <v>52</v>
@@ -3516,13 +3516,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{198DDAED-E1D3-421A-9A78-7D13A4837167}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView zoomScale="97" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" zoomScale="97" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -3539,106 +3539,106 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>307</v>
+      </c>
+      <c r="B2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C2" t="s">
         <v>58</v>
       </c>
-      <c r="B2" t="s">
-        <v>263</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>59</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>307</v>
+      </c>
+      <c r="B3" t="s">
+        <v>260</v>
+      </c>
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" t="s">
         <v>60</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B3" t="s">
-        <v>263</v>
-      </c>
-      <c r="C3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>307</v>
+      </c>
+      <c r="B4" t="s">
+        <v>279</v>
+      </c>
+      <c r="C4" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" t="s">
-        <v>282</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>281</v>
+      </c>
+      <c r="E4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>307</v>
+      </c>
+      <c r="B5" t="s">
+        <v>279</v>
+      </c>
+      <c r="C5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" t="s">
         <v>64</v>
       </c>
-      <c r="D4" t="s">
-        <v>284</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="E5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" t="s">
-        <v>282</v>
-      </c>
-      <c r="C5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D5" t="s">
-        <v>65</v>
-      </c>
-      <c r="E5" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>307</v>
+      </c>
+      <c r="B6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C6" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" t="s">
-        <v>283</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>68</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>307</v>
+      </c>
+      <c r="B7" t="s">
+        <v>280</v>
+      </c>
+      <c r="C7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" t="s">
+        <v>261</v>
+      </c>
+      <c r="E7" t="s">
         <v>69</v>
-      </c>
-      <c r="E6" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" t="s">
-        <v>283</v>
-      </c>
-      <c r="C7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D7" t="s">
-        <v>264</v>
-      </c>
-      <c r="E7" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -3651,12 +3651,12 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -3670,116 +3670,116 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
         <v>71</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>264</v>
+      </c>
+      <c r="D2" t="s">
         <v>72</v>
       </c>
-      <c r="C2" t="s">
-        <v>267</v>
-      </c>
-      <c r="D2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
       <c r="B3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" t="s">
+        <v>258</v>
+      </c>
+      <c r="D3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>74</v>
       </c>
-      <c r="C3" t="s">
-        <v>261</v>
-      </c>
-      <c r="D3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>75</v>
       </c>
-      <c r="B4" t="s">
-        <v>76</v>
-      </c>
       <c r="C4" s="6" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" t="s">
         <v>75</v>
       </c>
-      <c r="B5" t="s">
-        <v>76</v>
-      </c>
       <c r="C5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>78</v>
       </c>
-      <c r="D5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>79</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="D6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>268</v>
-      </c>
-      <c r="D6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>81</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>82</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>83</v>
       </c>
-      <c r="D7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>84</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="D8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" t="s">
         <v>85</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="D8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>84</v>
-      </c>
-      <c r="B9" t="s">
-        <v>85</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>86</v>
-      </c>
-      <c r="D9" t="s">
-        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -3793,12 +3793,12 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A2" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -3809,129 +3809,129 @@
         <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C2" t="s">
+        <v>268</v>
+      </c>
+      <c r="D2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>306</v>
+      </c>
+      <c r="B3" t="s">
+        <v>260</v>
+      </c>
+      <c r="C3" t="s">
+        <v>268</v>
+      </c>
+      <c r="D3" t="s">
         <v>89</v>
       </c>
-      <c r="B2" t="s">
-        <v>263</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="E3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>306</v>
+      </c>
+      <c r="B4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>306</v>
+      </c>
+      <c r="B5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>306</v>
+      </c>
+      <c r="B6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>306</v>
+      </c>
+      <c r="B7" t="s">
+        <v>269</v>
+      </c>
+      <c r="C7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E7" t="s">
         <v>271</v>
       </c>
-      <c r="D2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B3" t="s">
-        <v>263</v>
-      </c>
-      <c r="C3" t="s">
-        <v>271</v>
-      </c>
-      <c r="D3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E4" t="s">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>306</v>
+      </c>
+      <c r="B8" t="s">
+        <v>269</v>
+      </c>
+      <c r="C8" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D5" t="s">
-        <v>96</v>
-      </c>
-      <c r="E5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>89</v>
-      </c>
-      <c r="B6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C6" t="s">
-        <v>94</v>
-      </c>
-      <c r="D6" t="s">
-        <v>97</v>
-      </c>
-      <c r="E6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B7" t="s">
-        <v>272</v>
-      </c>
-      <c r="C7" t="s">
-        <v>100</v>
-      </c>
-      <c r="D7" t="s">
-        <v>101</v>
-      </c>
-      <c r="E7" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>89</v>
-      </c>
-      <c r="B8" t="s">
-        <v>272</v>
-      </c>
-      <c r="C8" t="s">
-        <v>100</v>
-      </c>
       <c r="D8" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -3947,9 +3947,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -3957,20 +3957,20 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -3983,240 +3983,240 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" t="s">
         <v>103</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>104</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
         <v>106</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>107</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>109</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>110</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B4" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="C4" t="s">
         <v>112</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>113</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B5" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="C5" t="s">
         <v>115</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>116</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B6" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="C6" t="s">
         <v>118</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>119</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B7" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="C7" t="s">
         <v>121</v>
       </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>122</v>
       </c>
-      <c r="C7" t="s">
+      <c r="B8" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="C8" t="s">
         <v>124</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>125</v>
       </c>
-      <c r="C8" t="s">
+      <c r="B9" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="C9" t="s">
         <v>127</v>
       </c>
-      <c r="B9" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>128</v>
       </c>
-      <c r="C9" t="s">
+      <c r="B10" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="C10" t="s">
         <v>130</v>
       </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>131</v>
       </c>
-      <c r="C10" t="s">
+      <c r="B11" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="C11" t="s">
         <v>133</v>
       </c>
-      <c r="B11" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>134</v>
       </c>
-      <c r="C11" t="s">
+      <c r="B12" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="C12" t="s">
         <v>136</v>
       </c>
-      <c r="B12" t="s">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>137</v>
       </c>
-      <c r="C12" t="s">
+      <c r="B13" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="C13" t="s">
         <v>139</v>
       </c>
-      <c r="B13" t="s">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>140</v>
       </c>
-      <c r="C13" t="s">
+      <c r="B14" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="C14" t="s">
         <v>142</v>
       </c>
-      <c r="B14" t="s">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>143</v>
       </c>
-      <c r="C14" t="s">
+      <c r="B15" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="C15" t="s">
         <v>145</v>
       </c>
-      <c r="B15" t="s">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>146</v>
       </c>
-      <c r="C15" t="s">
+      <c r="B16" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="C16" t="s">
         <v>148</v>
       </c>
-      <c r="B16" t="s">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>274</v>
+      </c>
+      <c r="B17" t="s">
         <v>149</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>275</v>
+      </c>
+      <c r="B18" t="s">
+        <v>151</v>
+      </c>
+      <c r="C18" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>276</v>
+      </c>
+      <c r="B19" t="s">
+        <v>153</v>
+      </c>
+      <c r="C19" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>277</v>
       </c>
-      <c r="B17" t="s">
-        <v>151</v>
-      </c>
-      <c r="C17" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="B20" t="s">
+        <v>155</v>
+      </c>
+      <c r="C20" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>278</v>
       </c>
-      <c r="B18" t="s">
-        <v>153</v>
-      </c>
-      <c r="C18" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>279</v>
-      </c>
-      <c r="B19" t="s">
-        <v>155</v>
-      </c>
-      <c r="C19" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>280</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>157</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>158</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>281</v>
-      </c>
-      <c r="B21" t="s">
-        <v>159</v>
-      </c>
-      <c r="C21" t="s">
-        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -4229,12 +4229,12 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -4245,61 +4245,61 @@
         <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>305</v>
+      </c>
+      <c r="B2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D2" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="E2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C3" t="s">
+        <v>284</v>
+      </c>
+      <c r="D3" t="s">
         <v>163</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>305</v>
+      </c>
+      <c r="B4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4" t="s">
+        <v>282</v>
+      </c>
+      <c r="D4" t="s">
         <v>164</v>
       </c>
-      <c r="C2" t="s">
-        <v>286</v>
-      </c>
-      <c r="D2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>163</v>
-      </c>
-      <c r="B3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C3" t="s">
-        <v>287</v>
-      </c>
-      <c r="D3" t="s">
-        <v>166</v>
-      </c>
-      <c r="E3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>163</v>
-      </c>
-      <c r="B4" t="s">
-        <v>164</v>
-      </c>
-      <c r="C4" t="s">
-        <v>285</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>167</v>
-      </c>
-      <c r="E4" t="s">
-        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -4315,237 +4315,237 @@
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B1" t="s">
         <v>25</v>
       </c>
       <c r="C1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>173</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>174</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B4" t="s">
         <v>176</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" t="s">
         <v>177</v>
       </c>
-      <c r="C3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>178</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>179</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="B6" t="s">
         <v>181</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C6" t="s">
         <v>182</v>
       </c>
-      <c r="C5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>183</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>184</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="B8" t="s">
         <v>186</v>
       </c>
-      <c r="B7" t="s">
-        <v>187</v>
-      </c>
-      <c r="C7" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>188</v>
-      </c>
-      <c r="B8" t="s">
-        <v>189</v>
-      </c>
       <c r="C8" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>24</v>
       </c>
       <c r="B9" t="s">
+        <v>187</v>
+      </c>
+      <c r="C9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>188</v>
+      </c>
+      <c r="B10" t="s">
+        <v>189</v>
+      </c>
+      <c r="C10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>190</v>
       </c>
-      <c r="C9" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="B11" t="s">
         <v>191</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C11" t="s">
         <v>192</v>
       </c>
-      <c r="C10" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>193</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>194</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="B13" t="s">
         <v>196</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C13" t="s">
         <v>197</v>
       </c>
-      <c r="C12" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>198</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>199</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="B15" t="s">
         <v>201</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C15" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>202</v>
       </c>
-      <c r="C14" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="B16" t="s">
         <v>203</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C16" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>204</v>
       </c>
-      <c r="C15" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="B17" t="s">
         <v>205</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C17" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>206</v>
       </c>
-      <c r="C16" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="B18" t="s">
         <v>207</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>208</v>
       </c>
-      <c r="C17" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="B19" t="s">
         <v>209</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C19" t="s">
         <v>210</v>
       </c>
-      <c r="C18" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>211</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>212</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="B21" t="s">
         <v>214</v>
       </c>
-      <c r="B20" t="s">
-        <v>215</v>
-      </c>
-      <c r="C20" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>216</v>
-      </c>
-      <c r="B21" t="s">
-        <v>217</v>
-      </c>
       <c r="C21" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>